<commit_message>
Update activity báo cáo
</commit_message>
<xml_diff>
--- a/Thiết kế/UseCases/4. Báo cáo.xlsx
+++ b/Thiết kế/UseCases/4. Báo cáo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Homework\CN Phan Mem\Homework\CNPM\Thiết kế\UseCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\CNPM\Thiết kế\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359AE259-A7B8-415C-87E8-01B8BD4064C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74428EE6-D901-4B44-8972-5D650B98D0ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DC4A1FAB-29E9-4CDF-AA87-E1C49E30A895}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DC4A1FAB-29E9-4CDF-AA87-E1C49E30A895}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>Use Case Number:</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>A4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -328,6 +331,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -336,21 +354,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -373,23 +376,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>122724</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>73904</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>122757</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>84819</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C29D627-B209-4737-9017-567BA3ED0657}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79938D4D-0557-4B93-AB81-F871F241B487}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -405,8 +408,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8436429" y="217714"/>
-          <a:ext cx="8809524" cy="7476190"/>
+          <a:off x="7724775" y="0"/>
+          <a:ext cx="8542857" cy="7247619"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -715,66 +718,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66CC78D9-3A50-4CE9-A19E-A78CD40F6C27}">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33:L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" style="3" customWidth="1"/>
-    <col min="2" max="3" width="39.6640625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="34.7109375" style="3" customWidth="1"/>
+    <col min="2" max="3" width="39.7109375" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="9"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="9"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="9"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -784,64 +787,64 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="15"/>
       <c r="B7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
+    <row r="8" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
       <c r="B9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
+    <row r="10" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
+    <row r="11" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
+    <row r="12" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
+      <c r="C14" s="15"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
       <c r="B15" s="6" t="s">
         <v>7</v>
       </c>
@@ -849,34 +852,34 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
       <c r="B16" s="7" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="7"/>
     </row>
-    <row r="17" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
+    <row r="17" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="10" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
       <c r="B20" s="6" t="s">
         <v>7</v>
       </c>
@@ -884,34 +887,34 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
+    <row r="21" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
       <c r="B21" s="7" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="7"/>
     </row>
-    <row r="22" spans="1:3" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
+    <row r="22" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
       <c r="B24" s="6" t="s">
         <v>37</v>
       </c>
       <c r="C24" s="7"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
       <c r="B25" s="6" t="s">
         <v>7</v>
       </c>
@@ -919,34 +922,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
+    <row r="26" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
       <c r="B26" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="7"/>
     </row>
-    <row r="27" spans="1:3" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+    <row r="27" spans="1:5" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
+      <c r="E27" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="15" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="8" t="s">
         <v>45</v>
       </c>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
       <c r="B30" s="6" t="s">
         <v>7</v>
       </c>
@@ -954,34 +960,34 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
+    <row r="31" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
       <c r="B31" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C31" s="7"/>
     </row>
-    <row r="32" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
+    <row r="32" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="13"/>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
-      <c r="B34" s="15" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="8" t="s">
         <v>44</v>
       </c>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="11"/>
       <c r="B35" s="6" t="s">
         <v>7</v>
       </c>
@@ -989,347 +995,347 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
+    <row r="36" spans="1:3" ht="33" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
       <c r="B36" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C36" s="7"/>
     </row>
-    <row r="37" spans="1:3" ht="50.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
+    <row r="37" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="14"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="10"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="15"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C40" s="9"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C41" s="9"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C41" s="14"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="9"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="14"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C43" s="9"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C43" s="14"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="9"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="14"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="9"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="14"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="9"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C46" s="14"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" s="13">
         <v>44158</v>
       </c>
-      <c r="C47" s="9"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C47" s="14"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="5"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>

</xml_diff>